<commit_message>
Updated data through 8/15
</commit_message>
<xml_diff>
--- a/Wordle Tracking v2.xlsx
+++ b/Wordle Tracking v2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riese\WordleTracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D08510A2-D4CB-4ED9-9049-68156D1CC0F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{260FB5ED-C17A-4F5A-90C9-D68659656902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="218">
   <si>
     <t>Date</t>
   </si>
@@ -524,6 +524,168 @@
   </si>
   <si>
     <t>AWFUL</t>
+  </si>
+  <si>
+    <t>BRINK</t>
+  </si>
+  <si>
+    <t>SMITE</t>
+  </si>
+  <si>
+    <t>BEADY</t>
+  </si>
+  <si>
+    <t>RUSTY</t>
+  </si>
+  <si>
+    <t>RETRO</t>
+  </si>
+  <si>
+    <t>DROLL</t>
+  </si>
+  <si>
+    <t>HUTCH</t>
+  </si>
+  <si>
+    <t>PINTO</t>
+  </si>
+  <si>
+    <t>EGRET</t>
+  </si>
+  <si>
+    <t>LILAC</t>
+  </si>
+  <si>
+    <t>SEVER</t>
+  </si>
+  <si>
+    <t>FIELD</t>
+  </si>
+  <si>
+    <t>FLUFF</t>
+  </si>
+  <si>
+    <t>AGAPE</t>
+  </si>
+  <si>
+    <t>VOICE</t>
+  </si>
+  <si>
+    <t>STEAD</t>
+  </si>
+  <si>
+    <t>BERTH</t>
+  </si>
+  <si>
+    <t>MADAM</t>
+  </si>
+  <si>
+    <t>NIGHT</t>
+  </si>
+  <si>
+    <t>BLAND</t>
+  </si>
+  <si>
+    <t>LIVER</t>
+  </si>
+  <si>
+    <t>WEDGE</t>
+  </si>
+  <si>
+    <t>ROOMY</t>
+  </si>
+  <si>
+    <t>WACKY</t>
+  </si>
+  <si>
+    <t>FLOCK</t>
+  </si>
+  <si>
+    <t>ANGRY</t>
+  </si>
+  <si>
+    <t>TRITE</t>
+  </si>
+  <si>
+    <t>APHID</t>
+  </si>
+  <si>
+    <t>TRYST</t>
+  </si>
+  <si>
+    <t>MIDGE</t>
+  </si>
+  <si>
+    <t>POWER</t>
+  </si>
+  <si>
+    <t>ELOPE</t>
+  </si>
+  <si>
+    <t>CINCH</t>
+  </si>
+  <si>
+    <t>MOTTO</t>
+  </si>
+  <si>
+    <t>STOMP</t>
+  </si>
+  <si>
+    <t>UPSET</t>
+  </si>
+  <si>
+    <t>BLUFF</t>
+  </si>
+  <si>
+    <t>GAWKY</t>
+  </si>
+  <si>
+    <t>CRAMP</t>
+  </si>
+  <si>
+    <t>QUART</t>
+  </si>
+  <si>
+    <t>COYLY</t>
+  </si>
+  <si>
+    <t>YOUTH</t>
+  </si>
+  <si>
+    <t>RHYME</t>
+  </si>
+  <si>
+    <t>BUGGY</t>
+  </si>
+  <si>
+    <t>ALIEN</t>
+  </si>
+  <si>
+    <t>SMEAR</t>
+  </si>
+  <si>
+    <t>UNFIT</t>
+  </si>
+  <si>
+    <t>PATTY</t>
+  </si>
+  <si>
+    <t>CLING</t>
+  </si>
+  <si>
+    <t>GLEAN</t>
+  </si>
+  <si>
+    <t>LABEL</t>
+  </si>
+  <si>
+    <t>HUNKY</t>
+  </si>
+  <si>
+    <t>KHAKI</t>
+  </si>
+  <si>
+    <t>POKER</t>
   </si>
 </sst>
 </file>
@@ -935,11 +1097,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N349"/>
+  <dimension ref="A1:N329"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H152" sqref="H152"/>
+      <pane ySplit="1" topLeftCell="A182" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D207" sqref="D207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5153,11 +5315,11 @@
     </row>
     <row r="131" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A131" s="3">
-        <f t="shared" ref="A131:A152" si="4">A130+1</f>
+        <f t="shared" ref="A131:A194" si="4">A130+1</f>
         <v>44348</v>
       </c>
       <c r="B131">
-        <f t="shared" ref="B131:B152" si="5">B130+1</f>
+        <f t="shared" ref="B131:B194" si="5">B130+1</f>
         <v>347</v>
       </c>
       <c r="C131" s="5" t="s">
@@ -5817,8 +5979,12 @@
       <c r="C152" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="D152" s="7"/>
-      <c r="E152" s="6"/>
+      <c r="D152" s="7">
+        <v>4</v>
+      </c>
+      <c r="E152" s="6">
+        <v>4</v>
+      </c>
       <c r="F152" s="6">
         <v>5</v>
       </c>
@@ -5830,10 +5996,26 @@
       <c r="L152" s="7"/>
     </row>
     <row r="153" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="C153" s="5"/>
-      <c r="D153" s="7"/>
-      <c r="E153" s="6"/>
-      <c r="F153" s="6"/>
+      <c r="A153" s="3">
+        <f t="shared" si="4"/>
+        <v>44370</v>
+      </c>
+      <c r="B153">
+        <f t="shared" si="5"/>
+        <v>369</v>
+      </c>
+      <c r="C153" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="D153" s="7">
+        <v>4</v>
+      </c>
+      <c r="E153" s="6">
+        <v>5</v>
+      </c>
+      <c r="F153" s="6">
+        <v>3</v>
+      </c>
       <c r="G153" s="7"/>
       <c r="H153" s="6"/>
       <c r="I153" s="7"/>
@@ -5842,10 +6024,26 @@
       <c r="L153" s="7"/>
     </row>
     <row r="154" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="C154" s="5"/>
-      <c r="D154" s="7"/>
-      <c r="E154" s="6"/>
-      <c r="F154" s="6"/>
+      <c r="A154" s="3">
+        <f t="shared" si="4"/>
+        <v>44371</v>
+      </c>
+      <c r="B154">
+        <f t="shared" si="5"/>
+        <v>370</v>
+      </c>
+      <c r="C154" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="D154" s="7">
+        <v>5</v>
+      </c>
+      <c r="E154" s="6">
+        <v>3</v>
+      </c>
+      <c r="F154" s="6">
+        <v>4</v>
+      </c>
       <c r="G154" s="7"/>
       <c r="H154" s="6"/>
       <c r="I154" s="7"/>
@@ -5854,10 +6052,24 @@
       <c r="L154" s="7"/>
     </row>
     <row r="155" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="C155" s="5"/>
-      <c r="D155" s="7"/>
+      <c r="A155" s="3">
+        <f t="shared" si="4"/>
+        <v>44372</v>
+      </c>
+      <c r="B155">
+        <f t="shared" si="5"/>
+        <v>371</v>
+      </c>
+      <c r="C155" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="D155" s="7">
+        <v>4</v>
+      </c>
       <c r="E155" s="6"/>
-      <c r="F155" s="6"/>
+      <c r="F155" s="6">
+        <v>4</v>
+      </c>
       <c r="G155" s="7"/>
       <c r="H155" s="6"/>
       <c r="I155" s="7"/>
@@ -5866,10 +6078,26 @@
       <c r="L155" s="7"/>
     </row>
     <row r="156" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="C156" s="5"/>
-      <c r="D156" s="7"/>
-      <c r="E156" s="6"/>
-      <c r="F156" s="6"/>
+      <c r="A156" s="3">
+        <f t="shared" si="4"/>
+        <v>44373</v>
+      </c>
+      <c r="B156">
+        <f t="shared" si="5"/>
+        <v>372</v>
+      </c>
+      <c r="C156" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="D156" s="7">
+        <v>4</v>
+      </c>
+      <c r="E156" s="6">
+        <v>3</v>
+      </c>
+      <c r="F156" s="6">
+        <v>4</v>
+      </c>
       <c r="G156" s="7"/>
       <c r="H156" s="6"/>
       <c r="I156" s="7"/>
@@ -5878,10 +6106,26 @@
       <c r="L156" s="7"/>
     </row>
     <row r="157" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="C157" s="5"/>
-      <c r="D157" s="7"/>
-      <c r="E157" s="6"/>
-      <c r="F157" s="6"/>
+      <c r="A157" s="3">
+        <f t="shared" si="4"/>
+        <v>44374</v>
+      </c>
+      <c r="B157">
+        <f t="shared" si="5"/>
+        <v>373</v>
+      </c>
+      <c r="C157" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="D157" s="7">
+        <v>5</v>
+      </c>
+      <c r="E157" s="6">
+        <v>3</v>
+      </c>
+      <c r="F157" s="6">
+        <v>4</v>
+      </c>
       <c r="G157" s="7"/>
       <c r="H157" s="6"/>
       <c r="I157" s="7"/>
@@ -5890,10 +6134,26 @@
       <c r="L157" s="7"/>
     </row>
     <row r="158" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="C158" s="5"/>
-      <c r="D158" s="7"/>
-      <c r="E158" s="6"/>
-      <c r="F158" s="6"/>
+      <c r="A158" s="3">
+        <f t="shared" si="4"/>
+        <v>44375</v>
+      </c>
+      <c r="B158">
+        <f t="shared" si="5"/>
+        <v>374</v>
+      </c>
+      <c r="C158" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="D158" s="7">
+        <v>3</v>
+      </c>
+      <c r="E158" s="6">
+        <v>4</v>
+      </c>
+      <c r="F158" s="6">
+        <v>3</v>
+      </c>
       <c r="G158" s="7"/>
       <c r="H158" s="6"/>
       <c r="I158" s="7"/>
@@ -5902,10 +6162,26 @@
       <c r="L158" s="7"/>
     </row>
     <row r="159" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="C159" s="5"/>
-      <c r="D159" s="7"/>
-      <c r="E159" s="6"/>
-      <c r="F159" s="6"/>
+      <c r="A159" s="3">
+        <f t="shared" si="4"/>
+        <v>44376</v>
+      </c>
+      <c r="B159">
+        <f t="shared" si="5"/>
+        <v>375</v>
+      </c>
+      <c r="C159" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="D159" s="7">
+        <v>4</v>
+      </c>
+      <c r="E159" s="6">
+        <v>3</v>
+      </c>
+      <c r="F159" s="6">
+        <v>5</v>
+      </c>
       <c r="G159" s="7"/>
       <c r="H159" s="6"/>
       <c r="I159" s="7"/>
@@ -5914,10 +6190,26 @@
       <c r="L159" s="7"/>
     </row>
     <row r="160" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="C160" s="5"/>
-      <c r="D160" s="7"/>
-      <c r="E160" s="6"/>
-      <c r="F160" s="6"/>
+      <c r="A160" s="3">
+        <f t="shared" si="4"/>
+        <v>44377</v>
+      </c>
+      <c r="B160">
+        <f t="shared" si="5"/>
+        <v>376</v>
+      </c>
+      <c r="C160" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="D160" s="7">
+        <v>6</v>
+      </c>
+      <c r="E160" s="6">
+        <v>5</v>
+      </c>
+      <c r="F160" s="6">
+        <v>5</v>
+      </c>
       <c r="G160" s="7"/>
       <c r="H160" s="6"/>
       <c r="I160" s="7"/>
@@ -5925,11 +6217,27 @@
       <c r="K160" s="7"/>
       <c r="L160" s="7"/>
     </row>
-    <row r="161" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C161" s="5"/>
-      <c r="D161" s="7"/>
-      <c r="E161" s="6"/>
-      <c r="F161" s="6"/>
+    <row r="161" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A161" s="3">
+        <f t="shared" si="4"/>
+        <v>44378</v>
+      </c>
+      <c r="B161">
+        <f t="shared" si="5"/>
+        <v>377</v>
+      </c>
+      <c r="C161" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="D161" s="7">
+        <v>3</v>
+      </c>
+      <c r="E161" s="6">
+        <v>4</v>
+      </c>
+      <c r="F161" s="6">
+        <v>5</v>
+      </c>
       <c r="G161" s="7"/>
       <c r="H161" s="6"/>
       <c r="I161" s="7"/>
@@ -5937,11 +6245,27 @@
       <c r="K161" s="7"/>
       <c r="L161" s="7"/>
     </row>
-    <row r="162" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C162" s="5"/>
-      <c r="D162" s="7"/>
-      <c r="E162" s="6"/>
-      <c r="F162" s="6"/>
+    <row r="162" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A162" s="3">
+        <f t="shared" si="4"/>
+        <v>44379</v>
+      </c>
+      <c r="B162">
+        <f t="shared" si="5"/>
+        <v>378</v>
+      </c>
+      <c r="C162" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="D162" s="7">
+        <v>5</v>
+      </c>
+      <c r="E162" s="6">
+        <v>4</v>
+      </c>
+      <c r="F162" s="6">
+        <v>3</v>
+      </c>
       <c r="G162" s="7"/>
       <c r="H162" s="6"/>
       <c r="I162" s="7"/>
@@ -5949,11 +6273,27 @@
       <c r="K162" s="7"/>
       <c r="L162" s="7"/>
     </row>
-    <row r="163" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C163" s="5"/>
-      <c r="D163" s="7"/>
-      <c r="E163" s="6"/>
-      <c r="F163" s="6"/>
+    <row r="163" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A163" s="3">
+        <f t="shared" si="4"/>
+        <v>44380</v>
+      </c>
+      <c r="B163">
+        <f t="shared" si="5"/>
+        <v>379</v>
+      </c>
+      <c r="C163" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="D163" s="7">
+        <v>3</v>
+      </c>
+      <c r="E163" s="6">
+        <v>4</v>
+      </c>
+      <c r="F163" s="6">
+        <v>4</v>
+      </c>
       <c r="G163" s="7"/>
       <c r="H163" s="6"/>
       <c r="I163" s="7"/>
@@ -5961,11 +6301,27 @@
       <c r="K163" s="7"/>
       <c r="L163" s="7"/>
     </row>
-    <row r="164" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C164" s="5"/>
-      <c r="D164" s="7"/>
-      <c r="E164" s="6"/>
-      <c r="F164" s="6"/>
+    <row r="164" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A164" s="3">
+        <f t="shared" si="4"/>
+        <v>44381</v>
+      </c>
+      <c r="B164">
+        <f t="shared" si="5"/>
+        <v>380</v>
+      </c>
+      <c r="C164" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="D164" s="7">
+        <v>5</v>
+      </c>
+      <c r="E164" s="6">
+        <v>4</v>
+      </c>
+      <c r="F164" s="6">
+        <v>5</v>
+      </c>
       <c r="G164" s="7"/>
       <c r="H164" s="6"/>
       <c r="I164" s="7"/>
@@ -5973,11 +6329,27 @@
       <c r="K164" s="7"/>
       <c r="L164" s="7"/>
     </row>
-    <row r="165" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C165" s="5"/>
-      <c r="D165" s="7"/>
-      <c r="E165" s="6"/>
-      <c r="F165" s="6"/>
+    <row r="165" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A165" s="3">
+        <f t="shared" si="4"/>
+        <v>44382</v>
+      </c>
+      <c r="B165">
+        <f t="shared" si="5"/>
+        <v>381</v>
+      </c>
+      <c r="C165" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="D165" s="7">
+        <v>4</v>
+      </c>
+      <c r="E165" s="6">
+        <v>3</v>
+      </c>
+      <c r="F165" s="6">
+        <v>4</v>
+      </c>
       <c r="G165" s="7"/>
       <c r="H165" s="6"/>
       <c r="I165" s="7"/>
@@ -5985,11 +6357,25 @@
       <c r="K165" s="7"/>
       <c r="L165" s="7"/>
     </row>
-    <row r="166" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C166" s="5"/>
-      <c r="D166" s="7"/>
+    <row r="166" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A166" s="3">
+        <f t="shared" si="4"/>
+        <v>44383</v>
+      </c>
+      <c r="B166">
+        <f t="shared" si="5"/>
+        <v>382</v>
+      </c>
+      <c r="C166" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="D166" s="7">
+        <v>6</v>
+      </c>
       <c r="E166" s="6"/>
-      <c r="F166" s="6"/>
+      <c r="F166" s="6">
+        <v>5</v>
+      </c>
       <c r="G166" s="7"/>
       <c r="H166" s="6"/>
       <c r="I166" s="7"/>
@@ -5997,11 +6383,27 @@
       <c r="K166" s="7"/>
       <c r="L166" s="7"/>
     </row>
-    <row r="167" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C167" s="5"/>
-      <c r="D167" s="7"/>
-      <c r="E167" s="6"/>
-      <c r="F167" s="6"/>
+    <row r="167" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A167" s="3">
+        <f t="shared" si="4"/>
+        <v>44384</v>
+      </c>
+      <c r="B167">
+        <f t="shared" si="5"/>
+        <v>383</v>
+      </c>
+      <c r="C167" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="D167" s="7">
+        <v>5</v>
+      </c>
+      <c r="E167" s="6">
+        <v>3</v>
+      </c>
+      <c r="F167" s="6">
+        <v>3</v>
+      </c>
       <c r="G167" s="7"/>
       <c r="H167" s="6"/>
       <c r="I167" s="7"/>
@@ -6009,11 +6411,27 @@
       <c r="K167" s="7"/>
       <c r="L167" s="7"/>
     </row>
-    <row r="168" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C168" s="5"/>
-      <c r="D168" s="7"/>
-      <c r="E168" s="6"/>
-      <c r="F168" s="6"/>
+    <row r="168" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A168" s="3">
+        <f t="shared" si="4"/>
+        <v>44385</v>
+      </c>
+      <c r="B168">
+        <f t="shared" si="5"/>
+        <v>384</v>
+      </c>
+      <c r="C168" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="D168" s="7">
+        <v>5</v>
+      </c>
+      <c r="E168" s="6">
+        <v>4</v>
+      </c>
+      <c r="F168" s="6">
+        <v>5</v>
+      </c>
       <c r="G168" s="7"/>
       <c r="H168" s="6"/>
       <c r="I168" s="7"/>
@@ -6021,11 +6439,27 @@
       <c r="K168" s="7"/>
       <c r="L168" s="7"/>
     </row>
-    <row r="169" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C169" s="5"/>
-      <c r="D169" s="7"/>
-      <c r="E169" s="6"/>
-      <c r="F169" s="6"/>
+    <row r="169" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A169" s="3">
+        <f t="shared" si="4"/>
+        <v>44386</v>
+      </c>
+      <c r="B169">
+        <f t="shared" si="5"/>
+        <v>385</v>
+      </c>
+      <c r="C169" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="D169" s="7">
+        <v>4</v>
+      </c>
+      <c r="E169" s="6">
+        <v>4</v>
+      </c>
+      <c r="F169" s="6">
+        <v>4</v>
+      </c>
       <c r="G169" s="7"/>
       <c r="H169" s="6"/>
       <c r="I169" s="7"/>
@@ -6033,11 +6467,27 @@
       <c r="K169" s="7"/>
       <c r="L169" s="7"/>
     </row>
-    <row r="170" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C170" s="5"/>
-      <c r="D170" s="7"/>
-      <c r="E170" s="6"/>
-      <c r="F170" s="6"/>
+    <row r="170" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A170" s="3">
+        <f t="shared" si="4"/>
+        <v>44387</v>
+      </c>
+      <c r="B170">
+        <f t="shared" si="5"/>
+        <v>386</v>
+      </c>
+      <c r="C170" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="D170" s="7">
+        <v>4</v>
+      </c>
+      <c r="E170" s="6">
+        <v>4</v>
+      </c>
+      <c r="F170" s="6">
+        <v>5</v>
+      </c>
       <c r="G170" s="7"/>
       <c r="H170" s="6"/>
       <c r="I170" s="7"/>
@@ -6045,11 +6495,27 @@
       <c r="K170" s="7"/>
       <c r="L170" s="7"/>
     </row>
-    <row r="171" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C171" s="5"/>
-      <c r="D171" s="7"/>
-      <c r="E171" s="6"/>
-      <c r="F171" s="6"/>
+    <row r="171" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A171" s="3">
+        <f t="shared" si="4"/>
+        <v>44388</v>
+      </c>
+      <c r="B171">
+        <f t="shared" si="5"/>
+        <v>387</v>
+      </c>
+      <c r="C171" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="D171" s="7">
+        <v>2</v>
+      </c>
+      <c r="E171" s="6">
+        <v>4</v>
+      </c>
+      <c r="F171" s="6">
+        <v>5</v>
+      </c>
       <c r="G171" s="7"/>
       <c r="H171" s="6"/>
       <c r="I171" s="7"/>
@@ -6057,11 +6523,27 @@
       <c r="K171" s="7"/>
       <c r="L171" s="7"/>
     </row>
-    <row r="172" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C172" s="5"/>
-      <c r="D172" s="7"/>
-      <c r="E172" s="6"/>
-      <c r="F172" s="6"/>
+    <row r="172" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A172" s="3">
+        <f t="shared" si="4"/>
+        <v>44389</v>
+      </c>
+      <c r="B172">
+        <f t="shared" si="5"/>
+        <v>388</v>
+      </c>
+      <c r="C172" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="D172" s="7">
+        <v>5</v>
+      </c>
+      <c r="E172" s="6">
+        <v>3</v>
+      </c>
+      <c r="F172" s="6">
+        <v>3</v>
+      </c>
       <c r="G172" s="7"/>
       <c r="H172" s="6"/>
       <c r="I172" s="7"/>
@@ -6069,11 +6551,27 @@
       <c r="K172" s="7"/>
       <c r="L172" s="7"/>
     </row>
-    <row r="173" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C173" s="5"/>
-      <c r="D173" s="7"/>
-      <c r="E173" s="6"/>
-      <c r="F173" s="6"/>
+    <row r="173" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A173" s="3">
+        <f t="shared" si="4"/>
+        <v>44390</v>
+      </c>
+      <c r="B173">
+        <f t="shared" si="5"/>
+        <v>389</v>
+      </c>
+      <c r="C173" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="D173" s="7">
+        <v>3</v>
+      </c>
+      <c r="E173" s="6">
+        <v>3</v>
+      </c>
+      <c r="F173" s="6">
+        <v>3</v>
+      </c>
       <c r="G173" s="7"/>
       <c r="H173" s="6"/>
       <c r="I173" s="7"/>
@@ -6081,11 +6579,27 @@
       <c r="K173" s="7"/>
       <c r="L173" s="7"/>
     </row>
-    <row r="174" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C174" s="5"/>
-      <c r="D174" s="7"/>
-      <c r="E174" s="6"/>
-      <c r="F174" s="6"/>
+    <row r="174" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A174" s="3">
+        <f t="shared" si="4"/>
+        <v>44391</v>
+      </c>
+      <c r="B174">
+        <f t="shared" si="5"/>
+        <v>390</v>
+      </c>
+      <c r="C174" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="D174" s="7">
+        <v>5</v>
+      </c>
+      <c r="E174" s="6">
+        <v>4</v>
+      </c>
+      <c r="F174" s="6">
+        <v>3</v>
+      </c>
       <c r="G174" s="7"/>
       <c r="H174" s="6"/>
       <c r="I174" s="7"/>
@@ -6093,11 +6607,27 @@
       <c r="K174" s="7"/>
       <c r="L174" s="7"/>
     </row>
-    <row r="175" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C175" s="5"/>
-      <c r="D175" s="7"/>
-      <c r="E175" s="6"/>
-      <c r="F175" s="6"/>
+    <row r="175" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A175" s="3">
+        <f t="shared" si="4"/>
+        <v>44392</v>
+      </c>
+      <c r="B175">
+        <f t="shared" si="5"/>
+        <v>391</v>
+      </c>
+      <c r="C175" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="D175" s="7">
+        <v>4</v>
+      </c>
+      <c r="E175" s="6">
+        <v>4</v>
+      </c>
+      <c r="F175" s="6">
+        <v>5</v>
+      </c>
       <c r="G175" s="7"/>
       <c r="H175" s="6"/>
       <c r="I175" s="7"/>
@@ -6105,11 +6635,27 @@
       <c r="K175" s="7"/>
       <c r="L175" s="7"/>
     </row>
-    <row r="176" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C176" s="5"/>
-      <c r="D176" s="7"/>
-      <c r="E176" s="6"/>
-      <c r="F176" s="6"/>
+    <row r="176" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A176" s="3">
+        <f t="shared" si="4"/>
+        <v>44393</v>
+      </c>
+      <c r="B176">
+        <f t="shared" si="5"/>
+        <v>392</v>
+      </c>
+      <c r="C176" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="D176" s="7">
+        <v>4</v>
+      </c>
+      <c r="E176" s="6">
+        <v>3</v>
+      </c>
+      <c r="F176" s="6">
+        <v>4</v>
+      </c>
       <c r="G176" s="7"/>
       <c r="H176" s="6"/>
       <c r="I176" s="7"/>
@@ -6117,11 +6663,27 @@
       <c r="K176" s="7"/>
       <c r="L176" s="7"/>
     </row>
-    <row r="177" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C177" s="5"/>
-      <c r="D177" s="7"/>
-      <c r="E177" s="6"/>
-      <c r="F177" s="6"/>
+    <row r="177" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A177" s="3">
+        <f t="shared" si="4"/>
+        <v>44394</v>
+      </c>
+      <c r="B177">
+        <f t="shared" si="5"/>
+        <v>393</v>
+      </c>
+      <c r="C177" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D177" s="7">
+        <v>4</v>
+      </c>
+      <c r="E177" s="6">
+        <v>3</v>
+      </c>
+      <c r="F177" s="6">
+        <v>4</v>
+      </c>
       <c r="G177" s="7"/>
       <c r="H177" s="6"/>
       <c r="I177" s="7"/>
@@ -6129,11 +6691,27 @@
       <c r="K177" s="7"/>
       <c r="L177" s="7"/>
     </row>
-    <row r="178" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C178" s="5"/>
-      <c r="D178" s="7"/>
-      <c r="E178" s="6"/>
-      <c r="F178" s="6"/>
+    <row r="178" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A178" s="3">
+        <f t="shared" si="4"/>
+        <v>44395</v>
+      </c>
+      <c r="B178">
+        <f t="shared" si="5"/>
+        <v>394</v>
+      </c>
+      <c r="C178" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="D178" s="7">
+        <v>2</v>
+      </c>
+      <c r="E178" s="6">
+        <v>2</v>
+      </c>
+      <c r="F178" s="6">
+        <v>5</v>
+      </c>
       <c r="G178" s="7"/>
       <c r="H178" s="6"/>
       <c r="I178" s="7"/>
@@ -6141,11 +6719,27 @@
       <c r="K178" s="7"/>
       <c r="L178" s="7"/>
     </row>
-    <row r="179" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C179" s="5"/>
-      <c r="D179" s="7"/>
-      <c r="E179" s="6"/>
-      <c r="F179" s="6"/>
+    <row r="179" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A179" s="3">
+        <f t="shared" si="4"/>
+        <v>44396</v>
+      </c>
+      <c r="B179">
+        <f t="shared" si="5"/>
+        <v>395</v>
+      </c>
+      <c r="C179" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="D179" s="7">
+        <v>4</v>
+      </c>
+      <c r="E179" s="6">
+        <v>5</v>
+      </c>
+      <c r="F179" s="6">
+        <v>3</v>
+      </c>
       <c r="G179" s="7"/>
       <c r="H179" s="6"/>
       <c r="I179" s="7"/>
@@ -6153,11 +6747,27 @@
       <c r="K179" s="7"/>
       <c r="L179" s="7"/>
     </row>
-    <row r="180" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C180" s="5"/>
-      <c r="D180" s="7"/>
-      <c r="E180" s="6"/>
-      <c r="F180" s="6"/>
+    <row r="180" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A180" s="3">
+        <f t="shared" si="4"/>
+        <v>44397</v>
+      </c>
+      <c r="B180">
+        <f t="shared" si="5"/>
+        <v>396</v>
+      </c>
+      <c r="C180" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="D180" s="7">
+        <v>4</v>
+      </c>
+      <c r="E180" s="6">
+        <v>3</v>
+      </c>
+      <c r="F180" s="6">
+        <v>3</v>
+      </c>
       <c r="G180" s="7"/>
       <c r="H180" s="6"/>
       <c r="I180" s="7"/>
@@ -6165,11 +6775,27 @@
       <c r="K180" s="7"/>
       <c r="L180" s="7"/>
     </row>
-    <row r="181" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C181" s="5"/>
-      <c r="D181" s="7"/>
-      <c r="E181" s="6"/>
-      <c r="F181" s="6"/>
+    <row r="181" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A181" s="3">
+        <f t="shared" si="4"/>
+        <v>44398</v>
+      </c>
+      <c r="B181">
+        <f t="shared" si="5"/>
+        <v>397</v>
+      </c>
+      <c r="C181" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="D181" s="7">
+        <v>4</v>
+      </c>
+      <c r="E181" s="6">
+        <v>4</v>
+      </c>
+      <c r="F181" s="6">
+        <v>4</v>
+      </c>
       <c r="G181" s="7"/>
       <c r="H181" s="6"/>
       <c r="I181" s="7"/>
@@ -6177,11 +6803,27 @@
       <c r="K181" s="7"/>
       <c r="L181" s="7"/>
     </row>
-    <row r="182" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C182" s="5"/>
-      <c r="D182" s="7"/>
-      <c r="E182" s="6"/>
-      <c r="F182" s="6"/>
+    <row r="182" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A182" s="3">
+        <f t="shared" si="4"/>
+        <v>44399</v>
+      </c>
+      <c r="B182">
+        <f t="shared" si="5"/>
+        <v>398</v>
+      </c>
+      <c r="C182" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="D182" s="7">
+        <v>4</v>
+      </c>
+      <c r="E182" s="6">
+        <v>3</v>
+      </c>
+      <c r="F182" s="6">
+        <v>5</v>
+      </c>
       <c r="G182" s="7"/>
       <c r="H182" s="6"/>
       <c r="I182" s="7"/>
@@ -6189,11 +6831,27 @@
       <c r="K182" s="7"/>
       <c r="L182" s="7"/>
     </row>
-    <row r="183" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C183" s="5"/>
-      <c r="D183" s="7"/>
-      <c r="E183" s="6"/>
-      <c r="F183" s="6"/>
+    <row r="183" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A183" s="3">
+        <f t="shared" si="4"/>
+        <v>44400</v>
+      </c>
+      <c r="B183">
+        <f t="shared" si="5"/>
+        <v>399</v>
+      </c>
+      <c r="C183" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="D183" s="7">
+        <v>4</v>
+      </c>
+      <c r="E183" s="6">
+        <v>4</v>
+      </c>
+      <c r="F183" s="6">
+        <v>3</v>
+      </c>
       <c r="G183" s="7"/>
       <c r="H183" s="6"/>
       <c r="I183" s="7"/>
@@ -6201,11 +6859,27 @@
       <c r="K183" s="7"/>
       <c r="L183" s="7"/>
     </row>
-    <row r="184" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C184" s="5"/>
-      <c r="D184" s="7"/>
-      <c r="E184" s="6"/>
-      <c r="F184" s="6"/>
+    <row r="184" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A184" s="3">
+        <f t="shared" si="4"/>
+        <v>44401</v>
+      </c>
+      <c r="B184">
+        <f t="shared" si="5"/>
+        <v>400</v>
+      </c>
+      <c r="C184" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="D184" s="7">
+        <v>5</v>
+      </c>
+      <c r="E184" s="6">
+        <v>4</v>
+      </c>
+      <c r="F184" s="6">
+        <v>5</v>
+      </c>
       <c r="G184" s="7"/>
       <c r="H184" s="6"/>
       <c r="I184" s="7"/>
@@ -6213,11 +6887,27 @@
       <c r="K184" s="7"/>
       <c r="L184" s="7"/>
     </row>
-    <row r="185" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C185" s="5"/>
-      <c r="D185" s="7"/>
-      <c r="E185" s="6"/>
-      <c r="F185" s="6"/>
+    <row r="185" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A185" s="3">
+        <f t="shared" si="4"/>
+        <v>44402</v>
+      </c>
+      <c r="B185">
+        <f t="shared" si="5"/>
+        <v>401</v>
+      </c>
+      <c r="C185" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="D185" s="7">
+        <v>5</v>
+      </c>
+      <c r="E185" s="6">
+        <v>5</v>
+      </c>
+      <c r="F185" s="6">
+        <v>4</v>
+      </c>
       <c r="G185" s="7"/>
       <c r="H185" s="6"/>
       <c r="I185" s="7"/>
@@ -6225,11 +6915,27 @@
       <c r="K185" s="7"/>
       <c r="L185" s="7"/>
     </row>
-    <row r="186" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C186" s="5"/>
-      <c r="D186" s="7"/>
-      <c r="E186" s="6"/>
-      <c r="F186" s="6"/>
+    <row r="186" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A186" s="3">
+        <f t="shared" si="4"/>
+        <v>44403</v>
+      </c>
+      <c r="B186">
+        <f t="shared" si="5"/>
+        <v>402</v>
+      </c>
+      <c r="C186" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="D186" s="7">
+        <v>5</v>
+      </c>
+      <c r="E186" s="6">
+        <v>5</v>
+      </c>
+      <c r="F186" s="6">
+        <v>4</v>
+      </c>
       <c r="G186" s="7"/>
       <c r="H186" s="6"/>
       <c r="I186" s="7"/>
@@ -6237,11 +6943,27 @@
       <c r="K186" s="7"/>
       <c r="L186" s="7"/>
     </row>
-    <row r="187" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C187" s="5"/>
-      <c r="D187" s="7"/>
-      <c r="E187" s="6"/>
-      <c r="F187" s="6"/>
+    <row r="187" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A187" s="3">
+        <f t="shared" si="4"/>
+        <v>44404</v>
+      </c>
+      <c r="B187">
+        <f t="shared" si="5"/>
+        <v>403</v>
+      </c>
+      <c r="C187" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="D187" s="7">
+        <v>4</v>
+      </c>
+      <c r="E187" s="6">
+        <v>4</v>
+      </c>
+      <c r="F187" s="6">
+        <v>5</v>
+      </c>
       <c r="G187" s="7"/>
       <c r="H187" s="6"/>
       <c r="I187" s="7"/>
@@ -6249,11 +6971,27 @@
       <c r="K187" s="7"/>
       <c r="L187" s="7"/>
     </row>
-    <row r="188" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C188" s="5"/>
-      <c r="D188" s="7"/>
-      <c r="E188" s="6"/>
-      <c r="F188" s="6"/>
+    <row r="188" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A188" s="3">
+        <f t="shared" si="4"/>
+        <v>44405</v>
+      </c>
+      <c r="B188">
+        <f t="shared" si="5"/>
+        <v>404</v>
+      </c>
+      <c r="C188" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="D188" s="7">
+        <v>4</v>
+      </c>
+      <c r="E188" s="6">
+        <v>4</v>
+      </c>
+      <c r="F188" s="6">
+        <v>3</v>
+      </c>
       <c r="G188" s="7"/>
       <c r="H188" s="6"/>
       <c r="I188" s="7"/>
@@ -6261,11 +6999,27 @@
       <c r="K188" s="7"/>
       <c r="L188" s="7"/>
     </row>
-    <row r="189" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C189" s="5"/>
-      <c r="D189" s="7"/>
-      <c r="E189" s="6"/>
-      <c r="F189" s="6"/>
+    <row r="189" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A189" s="3">
+        <f t="shared" si="4"/>
+        <v>44406</v>
+      </c>
+      <c r="B189">
+        <f t="shared" si="5"/>
+        <v>405</v>
+      </c>
+      <c r="C189" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="D189" s="7">
+        <v>4</v>
+      </c>
+      <c r="E189" s="6">
+        <v>4</v>
+      </c>
+      <c r="F189" s="6">
+        <v>3</v>
+      </c>
       <c r="G189" s="7"/>
       <c r="H189" s="6"/>
       <c r="I189" s="7"/>
@@ -6273,11 +7027,27 @@
       <c r="K189" s="7"/>
       <c r="L189" s="7"/>
     </row>
-    <row r="190" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C190" s="5"/>
-      <c r="D190" s="7"/>
-      <c r="E190" s="6"/>
-      <c r="F190" s="6"/>
+    <row r="190" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A190" s="3">
+        <f t="shared" si="4"/>
+        <v>44407</v>
+      </c>
+      <c r="B190">
+        <f t="shared" si="5"/>
+        <v>406</v>
+      </c>
+      <c r="C190" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="D190" s="7">
+        <v>4</v>
+      </c>
+      <c r="E190" s="6">
+        <v>3</v>
+      </c>
+      <c r="F190" s="6">
+        <v>5</v>
+      </c>
       <c r="G190" s="7"/>
       <c r="H190" s="6"/>
       <c r="I190" s="7"/>
@@ -6285,11 +7055,27 @@
       <c r="K190" s="7"/>
       <c r="L190" s="7"/>
     </row>
-    <row r="191" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C191" s="5"/>
-      <c r="D191" s="7"/>
-      <c r="E191" s="6"/>
-      <c r="F191" s="6"/>
+    <row r="191" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A191" s="3">
+        <f t="shared" si="4"/>
+        <v>44408</v>
+      </c>
+      <c r="B191">
+        <f t="shared" si="5"/>
+        <v>407</v>
+      </c>
+      <c r="C191" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="D191" s="7">
+        <v>5</v>
+      </c>
+      <c r="E191" s="6">
+        <v>4</v>
+      </c>
+      <c r="F191" s="6">
+        <v>4</v>
+      </c>
       <c r="G191" s="7"/>
       <c r="H191" s="6"/>
       <c r="I191" s="7"/>
@@ -6297,11 +7083,27 @@
       <c r="K191" s="7"/>
       <c r="L191" s="7"/>
     </row>
-    <row r="192" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C192" s="5"/>
-      <c r="D192" s="7"/>
-      <c r="E192" s="6"/>
-      <c r="F192" s="6"/>
+    <row r="192" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A192" s="3">
+        <f t="shared" si="4"/>
+        <v>44409</v>
+      </c>
+      <c r="B192">
+        <f t="shared" si="5"/>
+        <v>408</v>
+      </c>
+      <c r="C192" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D192" s="7">
+        <v>4</v>
+      </c>
+      <c r="E192" s="6">
+        <v>4</v>
+      </c>
+      <c r="F192" s="6">
+        <v>5</v>
+      </c>
       <c r="G192" s="7"/>
       <c r="H192" s="6"/>
       <c r="I192" s="7"/>
@@ -6309,11 +7111,27 @@
       <c r="K192" s="7"/>
       <c r="L192" s="7"/>
     </row>
-    <row r="193" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C193" s="5"/>
-      <c r="D193" s="7"/>
-      <c r="E193" s="6"/>
-      <c r="F193" s="6"/>
+    <row r="193" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A193" s="3">
+        <f t="shared" si="4"/>
+        <v>44410</v>
+      </c>
+      <c r="B193">
+        <f t="shared" si="5"/>
+        <v>409</v>
+      </c>
+      <c r="C193" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="D193" s="7">
+        <v>5</v>
+      </c>
+      <c r="E193" s="6">
+        <v>5</v>
+      </c>
+      <c r="F193" s="6">
+        <v>5</v>
+      </c>
       <c r="G193" s="7"/>
       <c r="H193" s="6"/>
       <c r="I193" s="7"/>
@@ -6321,11 +7139,27 @@
       <c r="K193" s="7"/>
       <c r="L193" s="7"/>
     </row>
-    <row r="194" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C194" s="5"/>
-      <c r="D194" s="7"/>
-      <c r="E194" s="6"/>
-      <c r="F194" s="6"/>
+    <row r="194" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A194" s="3">
+        <f t="shared" si="4"/>
+        <v>44411</v>
+      </c>
+      <c r="B194">
+        <f t="shared" si="5"/>
+        <v>410</v>
+      </c>
+      <c r="C194" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="D194" s="7">
+        <v>4</v>
+      </c>
+      <c r="E194" s="6">
+        <v>3</v>
+      </c>
+      <c r="F194" s="6">
+        <v>5</v>
+      </c>
       <c r="G194" s="7"/>
       <c r="H194" s="6"/>
       <c r="I194" s="7"/>
@@ -6333,11 +7167,27 @@
       <c r="K194" s="7"/>
       <c r="L194" s="7"/>
     </row>
-    <row r="195" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C195" s="5"/>
-      <c r="D195" s="7"/>
-      <c r="E195" s="6"/>
-      <c r="F195" s="6"/>
+    <row r="195" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A195" s="3">
+        <f t="shared" ref="A195:B206" si="6">A194+1</f>
+        <v>44412</v>
+      </c>
+      <c r="B195">
+        <f t="shared" si="6"/>
+        <v>411</v>
+      </c>
+      <c r="C195" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D195" s="7">
+        <v>4</v>
+      </c>
+      <c r="E195" s="6">
+        <v>2</v>
+      </c>
+      <c r="F195" s="6">
+        <v>4</v>
+      </c>
       <c r="G195" s="7"/>
       <c r="H195" s="6"/>
       <c r="I195" s="7"/>
@@ -6345,11 +7195,27 @@
       <c r="K195" s="7"/>
       <c r="L195" s="7"/>
     </row>
-    <row r="196" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C196" s="5"/>
-      <c r="D196" s="7"/>
-      <c r="E196" s="6"/>
-      <c r="F196" s="6"/>
+    <row r="196" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A196" s="3">
+        <f t="shared" si="6"/>
+        <v>44413</v>
+      </c>
+      <c r="B196">
+        <f t="shared" si="6"/>
+        <v>412</v>
+      </c>
+      <c r="C196" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="D196" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E196" s="6">
+        <v>4</v>
+      </c>
+      <c r="F196" s="6">
+        <v>4</v>
+      </c>
       <c r="G196" s="7"/>
       <c r="H196" s="6"/>
       <c r="I196" s="7"/>
@@ -6357,11 +7223,27 @@
       <c r="K196" s="7"/>
       <c r="L196" s="7"/>
     </row>
-    <row r="197" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C197" s="5"/>
-      <c r="D197" s="7"/>
-      <c r="E197" s="6"/>
-      <c r="F197" s="6"/>
+    <row r="197" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A197" s="3">
+        <f t="shared" si="6"/>
+        <v>44414</v>
+      </c>
+      <c r="B197">
+        <f t="shared" si="6"/>
+        <v>413</v>
+      </c>
+      <c r="C197" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="D197" s="7">
+        <v>4</v>
+      </c>
+      <c r="E197" s="6">
+        <v>4</v>
+      </c>
+      <c r="F197" s="6">
+        <v>3</v>
+      </c>
       <c r="G197" s="7"/>
       <c r="H197" s="6"/>
       <c r="I197" s="7"/>
@@ -6369,11 +7251,27 @@
       <c r="K197" s="7"/>
       <c r="L197" s="7"/>
     </row>
-    <row r="198" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C198" s="5"/>
-      <c r="D198" s="7"/>
-      <c r="E198" s="6"/>
-      <c r="F198" s="6"/>
+    <row r="198" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A198" s="3">
+        <f t="shared" si="6"/>
+        <v>44415</v>
+      </c>
+      <c r="B198">
+        <f t="shared" si="6"/>
+        <v>414</v>
+      </c>
+      <c r="C198" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="D198" s="7">
+        <v>4</v>
+      </c>
+      <c r="E198" s="6">
+        <v>5</v>
+      </c>
+      <c r="F198" s="6">
+        <v>3</v>
+      </c>
       <c r="G198" s="7"/>
       <c r="H198" s="6"/>
       <c r="I198" s="7"/>
@@ -6381,11 +7279,27 @@
       <c r="K198" s="7"/>
       <c r="L198" s="7"/>
     </row>
-    <row r="199" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C199" s="5"/>
-      <c r="D199" s="7"/>
-      <c r="E199" s="6"/>
-      <c r="F199" s="6"/>
+    <row r="199" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A199" s="3">
+        <f t="shared" si="6"/>
+        <v>44416</v>
+      </c>
+      <c r="B199">
+        <f t="shared" si="6"/>
+        <v>415</v>
+      </c>
+      <c r="C199" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="D199" s="7">
+        <v>4</v>
+      </c>
+      <c r="E199" s="6">
+        <v>3</v>
+      </c>
+      <c r="F199" s="6">
+        <v>4</v>
+      </c>
       <c r="G199" s="7"/>
       <c r="H199" s="6"/>
       <c r="I199" s="7"/>
@@ -6393,11 +7307,27 @@
       <c r="K199" s="7"/>
       <c r="L199" s="7"/>
     </row>
-    <row r="200" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C200" s="5"/>
-      <c r="D200" s="7"/>
-      <c r="E200" s="6"/>
-      <c r="F200" s="6"/>
+    <row r="200" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A200" s="3">
+        <f t="shared" si="6"/>
+        <v>44417</v>
+      </c>
+      <c r="B200">
+        <f t="shared" si="6"/>
+        <v>416</v>
+      </c>
+      <c r="C200" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="D200" s="7">
+        <v>4</v>
+      </c>
+      <c r="E200" s="6">
+        <v>4</v>
+      </c>
+      <c r="F200" s="6">
+        <v>4</v>
+      </c>
       <c r="G200" s="7"/>
       <c r="H200" s="6"/>
       <c r="I200" s="7"/>
@@ -6405,11 +7335,27 @@
       <c r="K200" s="7"/>
       <c r="L200" s="7"/>
     </row>
-    <row r="201" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C201" s="5"/>
-      <c r="D201" s="7"/>
-      <c r="E201" s="6"/>
-      <c r="F201" s="6"/>
+    <row r="201" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A201" s="3">
+        <f t="shared" si="6"/>
+        <v>44418</v>
+      </c>
+      <c r="B201">
+        <f t="shared" si="6"/>
+        <v>417</v>
+      </c>
+      <c r="C201" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="D201" s="7">
+        <v>5</v>
+      </c>
+      <c r="E201" s="6">
+        <v>6</v>
+      </c>
+      <c r="F201" s="6">
+        <v>6</v>
+      </c>
       <c r="G201" s="7"/>
       <c r="H201" s="6"/>
       <c r="I201" s="7"/>
@@ -6417,11 +7363,27 @@
       <c r="K201" s="7"/>
       <c r="L201" s="7"/>
     </row>
-    <row r="202" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C202" s="5"/>
-      <c r="D202" s="7"/>
-      <c r="E202" s="6"/>
-      <c r="F202" s="6"/>
+    <row r="202" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A202" s="3">
+        <f t="shared" si="6"/>
+        <v>44419</v>
+      </c>
+      <c r="B202">
+        <f t="shared" si="6"/>
+        <v>418</v>
+      </c>
+      <c r="C202" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="D202" s="7">
+        <v>4</v>
+      </c>
+      <c r="E202" s="6">
+        <v>4</v>
+      </c>
+      <c r="F202" s="6">
+        <v>4</v>
+      </c>
       <c r="G202" s="7"/>
       <c r="H202" s="6"/>
       <c r="I202" s="7"/>
@@ -6429,11 +7391,27 @@
       <c r="K202" s="7"/>
       <c r="L202" s="7"/>
     </row>
-    <row r="203" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C203" s="5"/>
-      <c r="D203" s="7"/>
-      <c r="E203" s="6"/>
-      <c r="F203" s="6"/>
+    <row r="203" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A203" s="3">
+        <f t="shared" si="6"/>
+        <v>44420</v>
+      </c>
+      <c r="B203">
+        <f t="shared" si="6"/>
+        <v>419</v>
+      </c>
+      <c r="C203" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="D203" s="7">
+        <v>4</v>
+      </c>
+      <c r="E203" s="6">
+        <v>5</v>
+      </c>
+      <c r="F203" s="6">
+        <v>4</v>
+      </c>
       <c r="G203" s="7"/>
       <c r="H203" s="6"/>
       <c r="I203" s="7"/>
@@ -6441,11 +7419,27 @@
       <c r="K203" s="7"/>
       <c r="L203" s="7"/>
     </row>
-    <row r="204" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C204" s="5"/>
-      <c r="D204" s="7"/>
-      <c r="E204" s="6"/>
-      <c r="F204" s="6"/>
+    <row r="204" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A204" s="3">
+        <f t="shared" si="6"/>
+        <v>44421</v>
+      </c>
+      <c r="B204">
+        <f t="shared" si="6"/>
+        <v>420</v>
+      </c>
+      <c r="C204" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="D204" s="7">
+        <v>3</v>
+      </c>
+      <c r="E204" s="6">
+        <v>4</v>
+      </c>
+      <c r="F204" s="6">
+        <v>4</v>
+      </c>
       <c r="G204" s="7"/>
       <c r="H204" s="6"/>
       <c r="I204" s="7"/>
@@ -6453,11 +7447,27 @@
       <c r="K204" s="7"/>
       <c r="L204" s="7"/>
     </row>
-    <row r="205" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C205" s="5"/>
-      <c r="D205" s="7"/>
-      <c r="E205" s="6"/>
-      <c r="F205" s="6"/>
+    <row r="205" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A205" s="3">
+        <f t="shared" si="6"/>
+        <v>44422</v>
+      </c>
+      <c r="B205">
+        <f t="shared" si="6"/>
+        <v>421</v>
+      </c>
+      <c r="C205" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="D205" s="7">
+        <v>5</v>
+      </c>
+      <c r="E205" s="6">
+        <v>3</v>
+      </c>
+      <c r="F205" s="6">
+        <v>5</v>
+      </c>
       <c r="G205" s="7"/>
       <c r="H205" s="6"/>
       <c r="I205" s="7"/>
@@ -6465,11 +7475,27 @@
       <c r="K205" s="7"/>
       <c r="L205" s="7"/>
     </row>
-    <row r="206" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C206" s="5"/>
-      <c r="D206" s="7"/>
-      <c r="E206" s="6"/>
-      <c r="F206" s="6"/>
+    <row r="206" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A206" s="3">
+        <f t="shared" si="6"/>
+        <v>44423</v>
+      </c>
+      <c r="B206">
+        <f t="shared" si="6"/>
+        <v>422</v>
+      </c>
+      <c r="C206" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="D206" s="7">
+        <v>4</v>
+      </c>
+      <c r="E206" s="6">
+        <v>4</v>
+      </c>
+      <c r="F206" s="6">
+        <v>4</v>
+      </c>
       <c r="G206" s="7"/>
       <c r="H206" s="6"/>
       <c r="I206" s="7"/>
@@ -6477,7 +7503,7 @@
       <c r="K206" s="7"/>
       <c r="L206" s="7"/>
     </row>
-    <row r="207" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C207" s="5"/>
       <c r="D207" s="7"/>
       <c r="E207" s="6"/>
@@ -6489,7 +7515,7 @@
       <c r="K207" s="7"/>
       <c r="L207" s="7"/>
     </row>
-    <row r="208" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C208" s="5"/>
       <c r="D208" s="7"/>
       <c r="E208" s="6"/>
@@ -7953,246 +8979,6 @@
       <c r="K329" s="7"/>
       <c r="L329" s="7"/>
     </row>
-    <row r="330" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C330" s="5"/>
-      <c r="D330" s="7"/>
-      <c r="E330" s="6"/>
-      <c r="F330" s="6"/>
-      <c r="G330" s="7"/>
-      <c r="H330" s="6"/>
-      <c r="I330" s="7"/>
-      <c r="J330" s="6"/>
-      <c r="K330" s="7"/>
-      <c r="L330" s="7"/>
-    </row>
-    <row r="331" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C331" s="5"/>
-      <c r="D331" s="7"/>
-      <c r="E331" s="6"/>
-      <c r="F331" s="6"/>
-      <c r="G331" s="7"/>
-      <c r="H331" s="6"/>
-      <c r="I331" s="7"/>
-      <c r="J331" s="6"/>
-      <c r="K331" s="7"/>
-      <c r="L331" s="7"/>
-    </row>
-    <row r="332" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C332" s="5"/>
-      <c r="D332" s="7"/>
-      <c r="E332" s="6"/>
-      <c r="F332" s="6"/>
-      <c r="G332" s="7"/>
-      <c r="H332" s="6"/>
-      <c r="I332" s="7"/>
-      <c r="J332" s="6"/>
-      <c r="K332" s="7"/>
-      <c r="L332" s="7"/>
-    </row>
-    <row r="333" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C333" s="5"/>
-      <c r="D333" s="7"/>
-      <c r="E333" s="6"/>
-      <c r="F333" s="6"/>
-      <c r="G333" s="7"/>
-      <c r="H333" s="6"/>
-      <c r="I333" s="7"/>
-      <c r="J333" s="6"/>
-      <c r="K333" s="7"/>
-      <c r="L333" s="7"/>
-    </row>
-    <row r="334" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C334" s="5"/>
-      <c r="D334" s="7"/>
-      <c r="E334" s="6"/>
-      <c r="F334" s="6"/>
-      <c r="G334" s="7"/>
-      <c r="H334" s="6"/>
-      <c r="I334" s="7"/>
-      <c r="J334" s="6"/>
-      <c r="K334" s="7"/>
-      <c r="L334" s="7"/>
-    </row>
-    <row r="335" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C335" s="5"/>
-      <c r="D335" s="7"/>
-      <c r="E335" s="6"/>
-      <c r="F335" s="6"/>
-      <c r="G335" s="7"/>
-      <c r="H335" s="6"/>
-      <c r="I335" s="7"/>
-      <c r="J335" s="6"/>
-      <c r="K335" s="7"/>
-      <c r="L335" s="7"/>
-    </row>
-    <row r="336" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C336" s="5"/>
-      <c r="D336" s="7"/>
-      <c r="E336" s="6"/>
-      <c r="F336" s="6"/>
-      <c r="G336" s="7"/>
-      <c r="H336" s="6"/>
-      <c r="I336" s="7"/>
-      <c r="J336" s="6"/>
-      <c r="K336" s="7"/>
-      <c r="L336" s="7"/>
-    </row>
-    <row r="337" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C337" s="5"/>
-      <c r="D337" s="7"/>
-      <c r="E337" s="6"/>
-      <c r="F337" s="6"/>
-      <c r="G337" s="7"/>
-      <c r="H337" s="6"/>
-      <c r="I337" s="7"/>
-      <c r="J337" s="6"/>
-      <c r="K337" s="7"/>
-      <c r="L337" s="7"/>
-    </row>
-    <row r="338" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C338" s="5"/>
-      <c r="D338" s="7"/>
-      <c r="E338" s="6"/>
-      <c r="F338" s="6"/>
-      <c r="G338" s="7"/>
-      <c r="H338" s="6"/>
-      <c r="I338" s="7"/>
-      <c r="J338" s="6"/>
-      <c r="K338" s="7"/>
-      <c r="L338" s="7"/>
-    </row>
-    <row r="339" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C339" s="5"/>
-      <c r="D339" s="7"/>
-      <c r="E339" s="6"/>
-      <c r="F339" s="6"/>
-      <c r="G339" s="7"/>
-      <c r="H339" s="6"/>
-      <c r="I339" s="7"/>
-      <c r="J339" s="6"/>
-      <c r="K339" s="7"/>
-      <c r="L339" s="7"/>
-    </row>
-    <row r="340" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C340" s="5"/>
-      <c r="D340" s="7"/>
-      <c r="E340" s="6"/>
-      <c r="F340" s="6"/>
-      <c r="G340" s="7"/>
-      <c r="H340" s="6"/>
-      <c r="I340" s="7"/>
-      <c r="J340" s="6"/>
-      <c r="K340" s="7"/>
-      <c r="L340" s="7"/>
-    </row>
-    <row r="341" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C341" s="5"/>
-      <c r="D341" s="7"/>
-      <c r="E341" s="6"/>
-      <c r="F341" s="6"/>
-      <c r="G341" s="7"/>
-      <c r="H341" s="6"/>
-      <c r="I341" s="7"/>
-      <c r="J341" s="6"/>
-      <c r="K341" s="7"/>
-      <c r="L341" s="7"/>
-    </row>
-    <row r="342" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C342" s="5"/>
-      <c r="D342" s="7"/>
-      <c r="E342" s="6"/>
-      <c r="F342" s="6"/>
-      <c r="G342" s="7"/>
-      <c r="H342" s="6"/>
-      <c r="I342" s="7"/>
-      <c r="J342" s="6"/>
-      <c r="K342" s="7"/>
-      <c r="L342" s="7"/>
-    </row>
-    <row r="343" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C343" s="5"/>
-      <c r="D343" s="7"/>
-      <c r="E343" s="6"/>
-      <c r="F343" s="6"/>
-      <c r="G343" s="7"/>
-      <c r="H343" s="6"/>
-      <c r="I343" s="7"/>
-      <c r="J343" s="6"/>
-      <c r="K343" s="7"/>
-      <c r="L343" s="7"/>
-    </row>
-    <row r="344" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C344" s="5"/>
-      <c r="D344" s="7"/>
-      <c r="E344" s="6"/>
-      <c r="F344" s="6"/>
-      <c r="G344" s="7"/>
-      <c r="H344" s="6"/>
-      <c r="I344" s="7"/>
-      <c r="J344" s="6"/>
-      <c r="K344" s="7"/>
-      <c r="L344" s="7"/>
-    </row>
-    <row r="345" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C345" s="5"/>
-      <c r="D345" s="7"/>
-      <c r="E345" s="6"/>
-      <c r="F345" s="6"/>
-      <c r="G345" s="7"/>
-      <c r="H345" s="6"/>
-      <c r="I345" s="7"/>
-      <c r="J345" s="6"/>
-      <c r="K345" s="7"/>
-      <c r="L345" s="7"/>
-    </row>
-    <row r="346" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C346" s="5"/>
-      <c r="D346" s="7"/>
-      <c r="E346" s="6"/>
-      <c r="F346" s="6"/>
-      <c r="G346" s="7"/>
-      <c r="H346" s="6"/>
-      <c r="I346" s="7"/>
-      <c r="J346" s="6"/>
-      <c r="K346" s="7"/>
-      <c r="L346" s="7"/>
-    </row>
-    <row r="347" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C347" s="5"/>
-      <c r="D347" s="7"/>
-      <c r="E347" s="6"/>
-      <c r="F347" s="6"/>
-      <c r="G347" s="7"/>
-      <c r="H347" s="6"/>
-      <c r="I347" s="7"/>
-      <c r="J347" s="6"/>
-      <c r="K347" s="7"/>
-      <c r="L347" s="7"/>
-    </row>
-    <row r="348" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C348" s="5"/>
-      <c r="D348" s="7"/>
-      <c r="E348" s="6"/>
-      <c r="F348" s="6"/>
-      <c r="G348" s="7"/>
-      <c r="H348" s="6"/>
-      <c r="I348" s="7"/>
-      <c r="J348" s="6"/>
-      <c r="K348" s="7"/>
-      <c r="L348" s="7"/>
-    </row>
-    <row r="349" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C349" s="5"/>
-      <c r="D349" s="7"/>
-      <c r="E349" s="6"/>
-      <c r="F349" s="6"/>
-      <c r="G349" s="7"/>
-      <c r="H349" s="6"/>
-      <c r="I349" s="7"/>
-      <c r="J349" s="6"/>
-      <c r="K349" s="7"/>
-      <c r="L349" s="7"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>